<commit_message>
- delete classification models - create parallel coordinates - delete old visualizations - update dashboard layout
</commit_message>
<xml_diff>
--- a/data/vegan_dataset.xlsx
+++ b/data/vegan_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fadb502cd9ab6c93/Documentos/GitHub/streamlit-data-vis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="652" documentId="13_ncr:1_{8636283F-4200-48B0-8C04-7D8A10333072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C31330C-0A15-4697-89D1-4AD899C8233D}"/>
+  <xr:revisionPtr revIDLastSave="654" documentId="13_ncr:1_{8636283F-4200-48B0-8C04-7D8A10333072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{614E5F6A-73EA-48A6-BEE0-528516185753}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10245" yWindow="5640" windowWidth="15915" windowHeight="9585" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUANTODECADACOISA" sheetId="6" r:id="rId1"/>
@@ -2363,9 +2363,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2403,7 +2403,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2509,7 +2509,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2651,7 +2651,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6651,8 +6651,8 @@
   <dimension ref="A1:AMJ277"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:O1"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E132" sqref="E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- new regex steps - option to choose between datasets - change vegan_dataset column to "Category"
</commit_message>
<xml_diff>
--- a/data/vegan_dataset.xlsx
+++ b/data/vegan_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fadb502cd9ab6c93/Documentos/GitHub/streamlit-data-vis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fadb502cd9ab6c93/Documentos/TCC/streamlit-data-vis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="654" documentId="13_ncr:1_{8636283F-4200-48B0-8C04-7D8A10333072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{614E5F6A-73EA-48A6-BEE0-528516185753}"/>
+  <xr:revisionPtr revIDLastSave="655" documentId="13_ncr:1_{8636283F-4200-48B0-8C04-7D8A10333072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{129BEA6F-D9B9-4ACC-9D93-40B7EDE6B8FD}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="5640" windowWidth="15915" windowHeight="9585" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="18285" windowHeight="12420" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUANTODECADACOISA" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="685">
   <si>
     <t>Porção</t>
   </si>
@@ -2109,6 +2109,9 @@
   </si>
   <si>
     <t>Total Fats</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
@@ -6650,9 +6653,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E132" sqref="E132"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6685,7 +6688,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>247</v>
+        <v>684</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>395</v>

</xml_diff>